<commit_message>
update version to v0.4
</commit_message>
<xml_diff>
--- a/src/test/resources/callApi/callApi.xlsx
+++ b/src/test/resources/callApi/callApi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\src\test\resources\callApi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2145D79B-3225-4C71-BCB6-46B152D9E4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C418A4E-8B17-4DAC-B428-CBE525FFE650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>TestCase</t>
   </si>
@@ -40,8 +40,6 @@
   },
   "body": {},
   "params": "",
-  "tests": {
-  },
   "store": [
     {
       "name": "name",
@@ -60,11 +58,47 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>saveProperties</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.json</t>
+    <t>echo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${name}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${age}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${job}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  "target": "https://task.hugang.io/time_entries.json",
+  "value": {
+    "method": "GET",
+    "headers": {
+      "X-Redmine-API-Key": "ed7449e623fc4b7bef6b0353cd59c5af652e2d66"
+    },
+    "body": {},
+    "params": "",
+    "store": [
+      {
+        "name": "name",
+        "value": "John"
+      },
+      {
+        "name": "age",
+        "responseKey": "total_count"
+      },
+      {
+        "name": "job",
+        "value": "Developer"
+      }
+    ]
+  }
+}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -161,7 +195,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -478,48 +512,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.25" style="2"/>
+    <col min="3" max="5" width="9.25" style="2"/>
+    <col min="6" max="6" width="59.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.25" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="393.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>